<commit_message>
get stack List with similars
</commit_message>
<xml_diff>
--- a/classico_django/classico_rest/Classico_django_RESTful URL.xlsx
+++ b/classico_django/classico_rest/Classico_django_RESTful URL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HunSeol/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HunSeol/django/classico-project/classico_django/classico_rest/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -146,16 +146,6 @@
   </si>
   <si>
     <t>{
- "Users": [{
-  "username": "",
-  "nickname": "",
-  "password": ""
- }]
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
  "password": "",
  "nickname": ""
 }</t>
@@ -195,6 +185,16 @@
   "",
   ""
  ]
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "Users": [{
+  "email": "",
+  "nickname": "",
+  "password": ""
+ }]
 }</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -308,41 +308,41 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -635,21 +635,21 @@
     <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="54.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="54.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -659,13 +659,13 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -675,13 +675,13 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -690,310 +690,310 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="13" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:14" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" s="13" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" s="13" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" s="12" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" s="13" customFormat="1" ht="54" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="D17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="8"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
+      <c r="B27" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>